<commit_message>
starting to update some vtt data
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20240904.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20240904.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0840A0-2EF5-4528-85D3-80D69CEDE897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63940DD-ED04-4C94-8EB4-918089A32A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="O&amp;M Costs" sheetId="1" r:id="rId1"/>
@@ -2377,7 +2377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -8495,64 +8495,64 @@
         <v>102</v>
       </c>
       <c r="R54" s="19">
-        <f>SUMIFS(R$2:R$49,$D$2:$D$49,$Q54,R$2:R$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="R54:Y57" si="43">SUMIFS(R$2:R$49,$D$2:$D$49,$Q54,R$2:R$49,"&lt;&gt;#N/A")</f>
         <v>39194</v>
       </c>
       <c r="S54" s="19">
-        <f>SUMIFS(S$2:S$49,$D$2:$D$49,$Q54,S$2:S$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>18370</v>
       </c>
       <c r="T54" s="19">
-        <f>SUMIFS(T$2:T$49,$D$2:$D$49,$Q54,T$2:T$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>163900</v>
       </c>
       <c r="U54" s="19">
-        <f>SUMIFS(U$2:U$49,$D$2:$D$49,$Q54,U$2:U$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>206316</v>
       </c>
       <c r="V54" s="19">
-        <f>SUMIFS(V$2:V$49,$D$2:$D$49,$Q54,V$2:V$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>484275</v>
       </c>
       <c r="W54" s="19">
-        <f>SUMIFS(W$2:W$49,$D$2:$D$49,$Q54,W$2:W$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>300581</v>
       </c>
       <c r="X54" s="19">
-        <f>SUMIFS(X$2:X$49,$D$2:$D$49,$Q54,X$2:X$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>312500</v>
       </c>
       <c r="Y54" s="35">
-        <f>SUMIFS(Y$2:Y$49,$D$2:$D$49,$Q54,Y$2:Y$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>1525136</v>
       </c>
       <c r="Z54" s="35"/>
       <c r="AA54" s="35">
-        <f>SUMIFS(AA$2:AA$49,$D$2:$D$49,$Q54,AA$2:AA$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="AA54:AG57" si="44">SUMIFS(AA$2:AA$49,$D$2:$D$49,$Q54,AA$2:AA$49,"&lt;&gt;#N/A")</f>
         <v>135396.36000000002</v>
       </c>
       <c r="AB54" s="21">
-        <f>SUMIFS(AB$2:AB$49,$D$2:$D$49,$Q54,AB$2:AB$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>9282</v>
       </c>
       <c r="AC54" s="21">
-        <f>SUMIFS(AC$2:AC$49,$D$2:$D$49,$Q54,AC$2:AC$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>26580</v>
       </c>
       <c r="AD54" s="21">
-        <f>SUMIFS(AD$2:AD$49,$D$2:$D$49,$Q54,AD$2:AD$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>22505.100000000002</v>
       </c>
       <c r="AE54" s="21">
-        <f>SUMIFS(AE$2:AE$49,$D$2:$D$49,$Q54,AE$2:AE$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>27000</v>
       </c>
       <c r="AF54" s="36">
-        <f>SUMIFS(AF$2:AF$49,$D$2:$D$49,$Q54,AF$2:AF$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>85367.1</v>
       </c>
       <c r="AG54" s="37">
-        <f>SUMIFS(AG$2:AG$49,$D$2:$D$49,$Q54,AG$2:AG$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>220763.45999999996</v>
       </c>
     </row>
@@ -8561,64 +8561,64 @@
         <v>97</v>
       </c>
       <c r="R55" s="19">
-        <f>SUMIFS(R$2:R$49,$D$2:$D$49,$Q55,R$2:R$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>13884</v>
       </c>
       <c r="S55" s="19">
-        <f>SUMIFS(S$2:S$49,$D$2:$D$49,$Q55,S$2:S$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>8350</v>
       </c>
       <c r="T55" s="19">
-        <f>SUMIFS(T$2:T$49,$D$2:$D$49,$Q55,T$2:T$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>48550</v>
       </c>
       <c r="U55" s="19">
-        <f>SUMIFS(U$2:U$49,$D$2:$D$49,$Q55,U$2:U$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>168804</v>
       </c>
       <c r="V55" s="19">
-        <f>SUMIFS(V$2:V$49,$D$2:$D$49,$Q55,V$2:V$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>249475</v>
       </c>
       <c r="W55" s="19">
-        <f>SUMIFS(W$2:W$49,$D$2:$D$49,$Q55,W$2:W$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>73556</v>
       </c>
       <c r="X55" s="19">
-        <f>SUMIFS(X$2:X$49,$D$2:$D$49,$Q55,X$2:X$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>125000</v>
       </c>
       <c r="Y55" s="35">
-        <f>SUMIFS(Y$2:Y$49,$D$2:$D$49,$Q55,Y$2:Y$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>687619</v>
       </c>
       <c r="Z55" s="35"/>
       <c r="AA55" s="35">
-        <f>SUMIFS(AA$2:AA$49,$D$2:$D$49,$Q55,AA$2:AA$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>55740.01999999999</v>
       </c>
       <c r="AB55" s="21">
-        <f>SUMIFS(AB$2:AB$49,$D$2:$D$49,$Q55,AB$2:AB$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>3276</v>
       </c>
       <c r="AC55" s="21">
-        <f>SUMIFS(AC$2:AC$49,$D$2:$D$49,$Q55,AC$2:AC$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>9240</v>
       </c>
       <c r="AD55" s="21">
-        <f>SUMIFS(AD$2:AD$49,$D$2:$D$49,$Q55,AD$2:AD$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>6961.51</v>
       </c>
       <c r="AE55" s="21">
-        <f>SUMIFS(AE$2:AE$49,$D$2:$D$49,$Q55,AE$2:AE$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>10800</v>
       </c>
       <c r="AF55" s="36">
-        <f>SUMIFS(AF$2:AF$49,$D$2:$D$49,$Q55,AF$2:AF$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>30277.510000000002</v>
       </c>
       <c r="AG55" s="37">
-        <f>SUMIFS(AG$2:AG$49,$D$2:$D$49,$Q55,AG$2:AG$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>86017.53</v>
       </c>
     </row>
@@ -8627,64 +8627,64 @@
         <v>100</v>
       </c>
       <c r="R56" s="19">
-        <f>SUMIFS(R$2:R$49,$D$2:$D$49,$Q56,R$2:R$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>6742</v>
       </c>
       <c r="S56" s="19">
-        <f>SUMIFS(S$2:S$49,$D$2:$D$49,$Q56,S$2:S$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>3340</v>
       </c>
       <c r="T56" s="19">
-        <f>SUMIFS(T$2:T$49,$D$2:$D$49,$Q56,T$2:T$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>17800</v>
       </c>
       <c r="U56" s="19">
-        <f>SUMIFS(U$2:U$49,$D$2:$D$49,$Q56,U$2:U$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>83360</v>
       </c>
       <c r="V56" s="19">
-        <f>SUMIFS(V$2:V$49,$D$2:$D$49,$Q56,V$2:V$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>117400</v>
       </c>
       <c r="W56" s="19">
-        <f>SUMIFS(W$2:W$49,$D$2:$D$49,$Q56,W$2:W$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>63801</v>
       </c>
       <c r="X56" s="19">
-        <f>SUMIFS(X$2:X$49,$D$2:$D$49,$Q56,X$2:X$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>50000</v>
       </c>
       <c r="Y56" s="35">
-        <f>SUMIFS(Y$2:Y$49,$D$2:$D$49,$Q56,Y$2:Y$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>342443</v>
       </c>
       <c r="Z56" s="35"/>
       <c r="AA56" s="35">
-        <f>SUMIFS(AA$2:AA$49,$D$2:$D$49,$Q56,AA$2:AA$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>27395.439999999999</v>
       </c>
       <c r="AB56" s="21">
-        <f>SUMIFS(AB$2:AB$49,$D$2:$D$49,$Q56,AB$2:AB$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>1456</v>
       </c>
       <c r="AC56" s="21">
-        <f>SUMIFS(AC$2:AC$49,$D$2:$D$49,$Q56,AC$2:AC$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>4620</v>
       </c>
       <c r="AD56" s="21">
-        <f>SUMIFS(AD$2:AD$49,$D$2:$D$49,$Q56,AD$2:AD$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>7141.6900000000005</v>
       </c>
       <c r="AE56" s="21">
-        <f>SUMIFS(AE$2:AE$49,$D$2:$D$49,$Q56,AE$2:AE$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>4320</v>
       </c>
       <c r="AF56" s="36">
-        <f>SUMIFS(AF$2:AF$49,$D$2:$D$49,$Q56,AF$2:AF$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>17537.690000000002</v>
       </c>
       <c r="AG56" s="37">
-        <f>SUMIFS(AG$2:AG$49,$D$2:$D$49,$Q56,AG$2:AG$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>44933.13</v>
       </c>
     </row>
@@ -8693,64 +8693,64 @@
         <v>101</v>
       </c>
       <c r="R57" s="19">
-        <f>SUMIFS(R$2:R$49,$D$2:$D$49,$Q57,R$2:R$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>9710</v>
       </c>
       <c r="S57" s="19">
-        <f>SUMIFS(S$2:S$49,$D$2:$D$49,$Q57,S$2:S$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>5010</v>
       </c>
       <c r="T57" s="19">
-        <f>SUMIFS(T$2:T$49,$D$2:$D$49,$Q57,T$2:T$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>29950</v>
       </c>
       <c r="U57" s="19">
-        <f>SUMIFS(U$2:U$49,$D$2:$D$49,$Q57,U$2:U$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>35428</v>
       </c>
       <c r="V57" s="19">
-        <f>SUMIFS(V$2:V$49,$D$2:$D$49,$Q57,V$2:V$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>85115</v>
       </c>
       <c r="W57" s="19">
-        <f>SUMIFS(W$2:W$49,$D$2:$D$49,$Q57,W$2:W$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>87259</v>
       </c>
       <c r="X57" s="19">
-        <f>SUMIFS(X$2:X$49,$D$2:$D$49,$Q57,X$2:X$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>62500</v>
       </c>
       <c r="Y57" s="35">
-        <f>SUMIFS(Y$2:Y$49,$D$2:$D$49,$Q57,Y$2:Y$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="43"/>
         <v>314972</v>
       </c>
       <c r="Z57" s="35"/>
       <c r="AA57" s="35">
-        <f>SUMIFS(AA$2:AA$49,$D$2:$D$49,$Q57,AA$2:AA$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>27655.260000000002</v>
       </c>
       <c r="AB57" s="21">
-        <f>SUMIFS(AB$2:AB$49,$D$2:$D$49,$Q57,AB$2:AB$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>2366</v>
       </c>
       <c r="AC57" s="21">
-        <f>SUMIFS(AC$2:AC$49,$D$2:$D$49,$Q57,AC$2:AC$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>5820</v>
       </c>
       <c r="AD57" s="21">
-        <f>SUMIFS(AD$2:AD$49,$D$2:$D$49,$Q57,AD$2:AD$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>4260.9500000000007</v>
       </c>
       <c r="AE57" s="21">
-        <f>SUMIFS(AE$2:AE$49,$D$2:$D$49,$Q57,AE$2:AE$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>8640</v>
       </c>
       <c r="AF57" s="36">
-        <f>SUMIFS(AF$2:AF$49,$D$2:$D$49,$Q57,AF$2:AF$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>21086.95</v>
       </c>
       <c r="AG57" s="37">
-        <f>SUMIFS(AG$2:AG$49,$D$2:$D$49,$Q57,AG$2:AG$49,"&lt;&gt;#N/A")</f>
+        <f t="shared" si="44"/>
         <v>48742.21</v>
       </c>
     </row>
@@ -8763,60 +8763,60 @@
         <v>48904</v>
       </c>
       <c r="S59" s="47">
-        <f t="shared" ref="S59:AG59" si="43">S54+S57</f>
+        <f t="shared" ref="S59:AG59" si="45">S54+S57</f>
         <v>23380</v>
       </c>
       <c r="T59" s="47">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>193850</v>
       </c>
       <c r="U59" s="47">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>241744</v>
       </c>
       <c r="V59" s="47">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>569390</v>
       </c>
       <c r="W59" s="47">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>387840</v>
       </c>
       <c r="X59" s="47">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>375000</v>
       </c>
       <c r="Y59" s="48">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>1840108</v>
       </c>
       <c r="Z59" s="48"/>
       <c r="AA59" s="48">
-        <f t="shared" ref="AA59" si="44">AA54+AA57</f>
+        <f t="shared" ref="AA59" si="46">AA54+AA57</f>
         <v>163051.62000000002</v>
       </c>
       <c r="AB59" s="49">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>11648</v>
       </c>
       <c r="AC59" s="49">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>32400</v>
       </c>
       <c r="AD59" s="49">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>26766.050000000003</v>
       </c>
       <c r="AE59" s="49">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>35640</v>
       </c>
       <c r="AF59" s="50">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>106454.05</v>
       </c>
       <c r="AG59" s="51">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>269505.67</v>
       </c>
     </row>
@@ -8829,60 +8829,60 @@
         <v>59820</v>
       </c>
       <c r="S60" s="47">
-        <f t="shared" ref="S60:AG60" si="45">SUM(S54:S56)</f>
+        <f t="shared" ref="S60:AG60" si="47">SUM(S54:S56)</f>
         <v>30060</v>
       </c>
       <c r="T60" s="47">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>230250</v>
       </c>
       <c r="U60" s="47">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>458480</v>
       </c>
       <c r="V60" s="47">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>851150</v>
       </c>
       <c r="W60" s="47">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>437938</v>
       </c>
       <c r="X60" s="47">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>487500</v>
       </c>
       <c r="Y60" s="48">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>2555198</v>
       </c>
       <c r="Z60" s="48"/>
       <c r="AA60" s="48">
-        <f t="shared" ref="AA60" si="46">SUM(AA54:AA56)</f>
+        <f t="shared" ref="AA60" si="48">SUM(AA54:AA56)</f>
         <v>218531.82</v>
       </c>
       <c r="AB60" s="49">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>14014</v>
       </c>
       <c r="AC60" s="49">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>40440</v>
       </c>
       <c r="AD60" s="49">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>36608.300000000003</v>
       </c>
       <c r="AE60" s="49">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>42120</v>
       </c>
       <c r="AF60" s="50">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>133182.30000000002</v>
       </c>
       <c r="AG60" s="51">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>351714.12</v>
       </c>
     </row>
@@ -8895,60 +8895,60 @@
         <v>10916</v>
       </c>
       <c r="S61" s="47">
-        <f t="shared" ref="S61:AG61" si="47">S60-S59</f>
+        <f t="shared" ref="S61:AG61" si="49">S60-S59</f>
         <v>6680</v>
       </c>
       <c r="T61" s="47">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>36400</v>
       </c>
       <c r="U61" s="47">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>216736</v>
       </c>
       <c r="V61" s="47">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>281760</v>
       </c>
       <c r="W61" s="47">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>50098</v>
       </c>
       <c r="X61" s="47">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>112500</v>
       </c>
       <c r="Y61" s="48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>715090</v>
       </c>
       <c r="Z61" s="48"/>
       <c r="AA61" s="48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>55480.199999999983</v>
       </c>
       <c r="AB61" s="49">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>2366</v>
       </c>
       <c r="AC61" s="49">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>8040</v>
       </c>
       <c r="AD61" s="49">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>9842.25</v>
       </c>
       <c r="AE61" s="49">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6480</v>
       </c>
       <c r="AF61" s="50">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>26728.250000000015</v>
       </c>
       <c r="AG61" s="51">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>82208.450000000012</v>
       </c>
     </row>
@@ -8961,60 +8961,60 @@
         <v>0.22321282512677901</v>
       </c>
       <c r="S62" s="52">
-        <f t="shared" ref="S62:AG62" si="48">S61/S59</f>
+        <f t="shared" ref="S62:AG62" si="50">S61/S59</f>
         <v>0.2857142857142857</v>
       </c>
       <c r="T62" s="52">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.18777405210214082</v>
       </c>
       <c r="U62" s="52">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.89655172413793105</v>
       </c>
       <c r="V62" s="52">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.49484536082474229</v>
       </c>
       <c r="W62" s="52">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.12917182343234324</v>
       </c>
       <c r="X62" s="52">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.3</v>
       </c>
       <c r="Y62" s="53">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.38861305966823684</v>
       </c>
       <c r="Z62" s="53"/>
       <c r="AA62" s="53">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.34026156869830532</v>
       </c>
       <c r="AB62" s="54">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.203125</v>
       </c>
       <c r="AC62" s="54">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.24814814814814815</v>
       </c>
       <c r="AD62" s="54">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.36771395106861116</v>
       </c>
       <c r="AE62" s="54">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="AF62" s="55">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.25107781244583943</v>
       </c>
       <c r="AG62" s="56">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0.30503421319484675</v>
       </c>
     </row>
@@ -15612,7 +15612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A5A9D4-9867-414A-873E-D5C500015276}">
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:G1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
created new iptds metadata file to be maintained moving forward for leaflet map
</commit_message>
<xml_diff>
--- a/data/om_costs/IPTDS O&M Costs 20240904.xlsx
+++ b/data/om_costs/IPTDS O&M Costs 20240904.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\om_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63940DD-ED04-4C94-8EB4-918089A32A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CD5516-DEE6-4070-BD1F-160EC61CC846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="O&amp;M Costs" sheetId="1" r:id="rId1"/>
@@ -2377,11 +2377,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -15612,7 +15612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A5A9D4-9867-414A-873E-D5C500015276}">
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:G1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>